<commit_message>
ML maxfr parameter scan and popvec decoding bias comparison
</commit_message>
<xml_diff>
--- a/goodness_of_fit_tables.xlsx
+++ b/goodness_of_fit_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim Alperen Tunc\.spyder-py3\bachelor_arbeit\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACD7C62-B5C4-4E22-99C3-25D83741DD26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F9B79C-AD67-4B66-A0E5-58F637341C81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="648" windowWidth="20748" windowHeight="11712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -224,9 +224,6 @@
     <t>Pop vector</t>
   </si>
   <si>
-    <t>BIC Nested</t>
-  </si>
-  <si>
     <t>uniform vs center only</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>61,726</t>
+  </si>
+  <si>
+    <t>BIC Nested HERE NOT APPLICABLE!!!!</t>
   </si>
 </sst>
 </file>
@@ -301,13 +301,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -591,14 +591,14 @@
   <dimension ref="A2:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
     <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.88671875" customWidth="1"/>
   </cols>
@@ -611,214 +611,214 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="5"/>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -826,91 +826,91 @@
         <v>60</v>
       </c>
       <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-9223</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-4371</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="2">
-        <v>-9223</v>
-      </c>
-      <c r="D18" s="2">
-        <v>-4371</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>